<commit_message>
Update logic when importing data to Excel file
</commit_message>
<xml_diff>
--- a/ConsoleAppFSharp/Template.xlsx
+++ b/ConsoleAppFSharp/Template.xlsx
@@ -27,12 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Sales</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>Sales Chart</t>
@@ -52,6 +49,15 @@
   <si>
     <t>Profit</t>
   </si>
+  <si>
+    <t>E-01</t>
+  </si>
+  <si>
+    <t>E-02</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
@@ -64,52 +70,80 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF0070C0"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="13.5"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Times New Roman Regular"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -450,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -478,28 +512,13 @@
         <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,26 +526,22 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -634,152 +649,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -787,27 +802,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1338,21 +1364,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.2109375" customWidth="1"/>
+    <col min="1" max="1" width="5.078125" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
     <col min="3" max="3" width="12.09375" customWidth="1"/>
     <col min="4" max="5" width="11.0078125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20" spans="1:20">
+    <row r="1" ht="23.2" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1360,205 +1386,310 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="K1" s="12" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="2" ht="19.2" spans="1:16">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-    </row>
-    <row r="2" ht="17.6" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+    </row>
+    <row r="3" ht="20" spans="1:16">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="C3" s="4">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
+        <v>30</v>
+      </c>
+      <c r="E3" s="5">
+        <v>100</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+    </row>
+    <row r="4" ht="20" spans="1:16">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5">
+        <v>40</v>
+      </c>
+      <c r="E4" s="5">
+        <v>100</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+    </row>
+    <row r="5" ht="19.2" spans="1:16">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8">
+        <f>SUM(C3:C4)</f>
+        <v>30</v>
+      </c>
+      <c r="D5" s="8">
+        <f>SUM(D3:D4)</f>
+        <v>70</v>
+      </c>
+      <c r="E5" s="8">
+        <f>SUM(E3:E4)</f>
+        <v>200</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" ht="17.6" spans="1:5">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" ht="17.6" spans="1:5">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="K1:T1"/>
+    <mergeCell ref="G1:P1"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>